<commit_message>
adding new testcases to registeration module
</commit_message>
<xml_diff>
--- a/Testing/Test Cases/Registeration TC.xlsx
+++ b/Testing/Test Cases/Registeration TC.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23010" windowHeight="8460"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="8460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="212">
   <si>
     <t>Project Name:</t>
   </si>
@@ -942,6 +942,104 @@
   </si>
   <si>
     <t>BANK_SYS_TC_Reg_R047</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Reg_R048</t>
+  </si>
+  <si>
+    <t>Validate that all fields are required expect staff id 
+in case of customer registeration.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- leave username textfield empty .
+2- enter password in the textfield password .
+3- enter confirm password in the textfield confirm password .
+4- enter national ID in the textfield national ID .
+5- enter email in the textfield email .
+6- enter phone in the textfield phone .
+7- leave staff id not selected .
+8-leave staff ID textfield empty.
+9- press on the button Register.
+</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Reg_R049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-user name : khadijaMostafa 
+2- passsword : deja&amp;123&amp;
+3- confirm password : deja&amp;123&amp;
+4- national ID : 12345678912345
+5- email : khadija.mostafa@gmail.com
+6- phone :01284751820
+7- Staff id : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- enter username in the textfield username .
+2- enter password in the textfield password .
+3- enter confirm password in the textfield confirm password .
+4- enter national ID in the textfield national ID .
+5- enter email in the textfield email .
+6- enter phone in the textfield phone .
+7-select staff id  .
+8-leave staff ID textfield empty.
+9- press on the button Register.
+10- enter the verification code.
+</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Reg_R050</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Reg_R051</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Reg_R032</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Reg_R031</t>
+  </si>
+  <si>
+    <t>Validate that all fields are required 
+in case of admin registeration.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-user name :
+2- passsword : deja&amp;123&amp;
+3- confirm password : deja&amp;123&amp;
+4- national ID : 12345678912345
+5- email : khadija.mostafa@gmail.com
+6- phone :01284751820
+</t>
+  </si>
+  <si>
+    <t>1-user name : khadijaMostafa 
+2- passsword : deja&amp;123&amp;
+3- confirm password : deja&amp;123&amp;
+4- national ID : 12345678912345
+5- email : khadija.mostafa@gmail.com
+6- phone :01284751820
+7- Staff id : 123457</t>
+  </si>
+  <si>
+    <t>1- enter username in the textfield username .
+2- enter password in the textfield password .
+3- enter confirm password in the textfield confirm password .
+4- enter national ID in the textfield national ID .
+5- enter email in the textfield email .
+6- enter phone in the textfield phone .
+7-select staff id  .
+8-eneter staff ID in the textfield staff id .
+9- press on the button Register.
+10- enter the verification code.</t>
+  </si>
+  <si>
+    <t>validate that no availability to register with 
+an exist customer data (customer register twice ).</t>
+  </si>
+  <si>
+    <t>validate that no availability to register with 
+an exist admin data (admin register twice).</t>
   </si>
 </sst>
 </file>
@@ -1455,10 +1553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L55"/>
+  <dimension ref="A1:L59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="A8" activeCellId="7" sqref="A1:XFD1 A2:XFD2 A3:XFD3 A4:XFD4 A5:XFD5 A6:XFD6 A7:XFD7 A8:XFD8"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2929,6 +3027,122 @@
         <v>25</v>
       </c>
     </row>
+    <row r="56" spans="1:10" ht="180" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>204</v>
+      </c>
+      <c r="B56" t="s">
+        <v>196</v>
+      </c>
+      <c r="C56" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="D56" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="E56" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="F56" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="H56" t="s">
+        <v>23</v>
+      </c>
+      <c r="I56" t="s">
+        <v>24</v>
+      </c>
+      <c r="J56" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="180" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>205</v>
+      </c>
+      <c r="B57" t="s">
+        <v>199</v>
+      </c>
+      <c r="C57" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="D57" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="E57" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="F57" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="H57" t="s">
+        <v>23</v>
+      </c>
+      <c r="I57" t="s">
+        <v>24</v>
+      </c>
+      <c r="J57" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="B58" t="s">
+        <v>202</v>
+      </c>
+      <c r="C58" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="D58" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="E58" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="F58" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="H58" t="s">
+        <v>23</v>
+      </c>
+      <c r="I58" t="s">
+        <v>24</v>
+      </c>
+      <c r="J58" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="B59" t="s">
+        <v>203</v>
+      </c>
+      <c r="C59" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="D59" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="E59" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="F59" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="H59" t="s">
+        <v>23</v>
+      </c>
+      <c r="I59" t="s">
+        <v>24</v>
+      </c>
+      <c r="J59" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B5:K5"/>

</xml_diff>

<commit_message>
update registeration form test cases
</commit_message>
<xml_diff>
--- a/Testing/Test Cases/Registeration TC.xlsx
+++ b/Testing/Test Cases/Registeration TC.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Internet-Banking-System\Testing\Test Cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\iti\project managment\coding\Internet-Banking-System\Testing\Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="212">
   <si>
     <t>Project Name:</t>
   </si>
@@ -766,6 +766,10 @@
   <si>
     <t>validate that staff ID Field shall not
 accept length 7.</t>
+  </si>
+  <si>
+    <t>validate that customer phone Field shall 
+accept length 6.</t>
   </si>
   <si>
     <t>validate that customer phone Field shall 
@@ -940,14 +944,108 @@
     <t>BANK_SYS_TC_Reg_R047</t>
   </si>
   <si>
-    <t>validate that staff ID Field shall 
-accept length 6.</t>
+    <t>BANK_SYS_TC_Reg_R048</t>
+  </si>
+  <si>
+    <t>Validate that all fields are required expect staff id 
+in case of customer registeration.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- leave username textfield empty .
+2- enter password in the textfield password .
+3- enter confirm password in the textfield confirm password .
+4- enter national ID in the textfield national ID .
+5- enter email in the textfield email .
+6- enter phone in the textfield phone .
+7- leave staff id not selected .
+8-leave staff ID textfield empty.
+9- press on the button Register.
+</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Reg_R049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-user name : khadijaMostafa 
+2- passsword : deja&amp;123&amp;
+3- confirm password : deja&amp;123&amp;
+4- national ID : 12345678912345
+5- email : khadija.mostafa@gmail.com
+6- phone :01284751820
+7- Staff id : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- enter username in the textfield username .
+2- enter password in the textfield password .
+3- enter confirm password in the textfield confirm password .
+4- enter national ID in the textfield national ID .
+5- enter email in the textfield email .
+6- enter phone in the textfield phone .
+7-select staff id  .
+8-leave staff ID textfield empty.
+9- press on the button Register.
+10- enter the verification code.
+</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Reg_R050</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Reg_R051</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Reg_R032</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Reg_R031</t>
+  </si>
+  <si>
+    <t>Validate that all fields are required 
+in case of admin registeration.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-user name :
+2- passsword : deja&amp;123&amp;
+3- confirm password : deja&amp;123&amp;
+4- national ID : 12345678912345
+5- email : khadija.mostafa@gmail.com
+6- phone :01284751820
+</t>
+  </si>
+  <si>
+    <t>1-user name : khadijaMostafa 
+2- passsword : deja&amp;123&amp;
+3- confirm password : deja&amp;123&amp;
+4- national ID : 12345678912345
+5- email : khadija.mostafa@gmail.com
+6- phone :01284751820
+7- Staff id : 123457</t>
+  </si>
+  <si>
+    <t>1- enter username in the textfield username .
+2- enter password in the textfield password .
+3- enter confirm password in the textfield confirm password .
+4- enter national ID in the textfield national ID .
+5- enter email in the textfield email .
+6- enter phone in the textfield phone .
+7-select staff id  .
+8-eneter staff ID in the textfield staff id .
+9- press on the button Register.
+10- enter the verification code.</t>
+  </si>
+  <si>
+    <t>validate that no availability to register with 
+an exist customer data (customer register twice ).</t>
+  </si>
+  <si>
+    <t>validate that no availability to register with 
+an exist admin data (admin register twice).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1455,10 +1553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L55"/>
+  <dimension ref="A1:L59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2557,7 +2655,7 @@
         <v>143</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C43" s="18" t="s">
         <v>144</v>
@@ -2586,7 +2684,7 @@
         <v>143</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C44" s="18" t="s">
         <v>145</v>
@@ -2615,7 +2713,7 @@
         <v>143</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C45" s="18" t="s">
         <v>146</v>
@@ -2644,16 +2742,16 @@
         <v>147</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C46" s="18" t="s">
         <v>161</v>
       </c>
       <c r="D46" s="18" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E46" s="18" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F46" s="18" t="s">
         <v>76</v>
@@ -2673,19 +2771,19 @@
         <v>147</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C47" s="18" t="s">
-        <v>195</v>
+        <v>162</v>
       </c>
       <c r="D47" s="18" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E47" s="18" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F47" s="18" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H47" s="20" t="s">
         <v>23</v>
@@ -2702,19 +2800,19 @@
         <v>147</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C48" s="18" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E48" s="18" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F48" s="18" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H48" s="20" t="s">
         <v>23</v>
@@ -2731,16 +2829,16 @@
         <v>147</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D49" s="18" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E49" s="18" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F49" s="18" t="s">
         <v>76</v>
@@ -2760,16 +2858,16 @@
         <v>147</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D50" s="18" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E50" s="18" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F50" s="18" t="s">
         <v>76</v>
@@ -2789,19 +2887,19 @@
         <v>27</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C51" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="D51" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="E51" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="D51" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="E51" s="18" t="s">
-        <v>169</v>
-      </c>
       <c r="F51" s="18" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H51" s="20" t="s">
         <v>23</v>
@@ -2815,22 +2913,22 @@
     </row>
     <row r="52" spans="1:10" ht="177" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D52" s="18" t="s">
         <v>45</v>
       </c>
       <c r="E52" s="18" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F52" s="18" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H52" s="20" t="s">
         <v>23</v>
@@ -2844,19 +2942,19 @@
     </row>
     <row r="53" spans="1:10" ht="177" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B53" s="19" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C53" s="18" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D53" s="18" t="s">
         <v>45</v>
       </c>
       <c r="E53" s="18" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F53" s="18" t="s">
         <v>76</v>
@@ -2873,22 +2971,22 @@
     </row>
     <row r="54" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B54" s="19" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C54" s="18" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D54" s="18" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E54" s="18" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F54" s="18" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H54" s="20" t="s">
         <v>23</v>
@@ -2902,19 +3000,19 @@
     </row>
     <row r="55" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B55" s="19" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C55" s="18" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D55" s="18" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E55" s="18" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F55" s="18" t="s">
         <v>76</v>
@@ -2926,6 +3024,122 @@
         <v>24</v>
       </c>
       <c r="J55" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="180" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>204</v>
+      </c>
+      <c r="B56" t="s">
+        <v>196</v>
+      </c>
+      <c r="C56" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="D56" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="E56" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="F56" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="H56" t="s">
+        <v>23</v>
+      </c>
+      <c r="I56" t="s">
+        <v>24</v>
+      </c>
+      <c r="J56" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="180" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>205</v>
+      </c>
+      <c r="B57" t="s">
+        <v>199</v>
+      </c>
+      <c r="C57" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="D57" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="E57" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="F57" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="H57" t="s">
+        <v>23</v>
+      </c>
+      <c r="I57" t="s">
+        <v>24</v>
+      </c>
+      <c r="J57" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="B58" t="s">
+        <v>202</v>
+      </c>
+      <c r="C58" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="D58" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="E58" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="F58" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="H58" t="s">
+        <v>23</v>
+      </c>
+      <c r="I58" t="s">
+        <v>24</v>
+      </c>
+      <c r="J58" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="B59" t="s">
+        <v>203</v>
+      </c>
+      <c r="C59" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="D59" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="E59" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="F59" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="H59" t="s">
+        <v>23</v>
+      </c>
+      <c r="I59" t="s">
+        <v>24</v>
+      </c>
+      <c r="J59" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update registeration testcases with the updates of the error mesage
</commit_message>
<xml_diff>
--- a/Testing/Test Cases/Registeration TC.xlsx
+++ b/Testing/Test Cases/Registeration TC.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\iti\project managment\coding\Internet-Banking-System\Testing\Test Cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\iti\project managment\for srs and siq and registeration update\Internet-Banking-System\Testing\Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="219">
   <si>
     <t>Project Name:</t>
   </si>
@@ -167,32 +167,6 @@
     <t>BANK_SYS_TC_Reg_R004</t>
   </si>
   <si>
-    <t xml:space="preserve">
-error messgae in the form of pop up shall be displayed with context" You have entered an invalid format of data, 
-Please try again." with ok button and close icon. 
-</t>
-  </si>
-  <si>
-    <t>validate that customer remain in the same page after 
-press on ok button in any  error message displayed .</t>
-  </si>
-  <si>
-    <t>1- enter username in the textfield username .
-2- enter password in the textfield password .
-3- enter confirm password in the textfield confirm password .
-4- enter national ID in the textfield national ID .
-5- enter email in the textfield email .
-6- enter phone in the textfield phone .
-7- leave staff id not selected .
-8-leave staff ID textfield empty.
-9- press on the button Register.
-10- click on ok in the pop up message .</t>
-  </si>
-  <si>
-    <t>error message shall be disappeared and cst 
-shall be remain in the registeration page .</t>
-  </si>
-  <si>
     <t xml:space="preserve">1-user name : KhadijaMostafa93
 2- passsword : deja&amp;123&amp;
 3- confirm password : deja&amp;123&amp;
@@ -221,14 +195,6 @@
     <t>validate that Username field shallnot  accept special characters  .</t>
   </si>
   <si>
-    <t>1-user name : KhadijaMostafa933333333333333333333333333333333333333333333333333
-2- passsword : deja&amp;123&amp;
-3- confirm password : deja&amp;123&amp;
-4- national ID : 12345678912345
-5- email : khadija.mostafa@gmail.com
-6- phone :01284751821</t>
-  </si>
-  <si>
     <t>BANK_SYS_TC_Reg_R005</t>
   </si>
   <si>
@@ -242,39 +208,7 @@
 &amp; BANK_SYS_SRS_Reg_R024</t>
   </si>
   <si>
-    <t xml:space="preserve">
- BANK_SYS_SRS_Reg_R029</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
- BANK_SYS_SRS_Reg_R030</t>
-  </si>
-  <si>
     <t>BANK_SYS_TC_Reg_R007</t>
-  </si>
-  <si>
-    <t>validate that customer remain in the same page after 
-press close icon in any  error message displayed .</t>
-  </si>
-  <si>
-    <t>1-user name : KhadijaMostafa933333333333333333333333333333333333333333333333333
-2- passsword : deja&amp;123&amp;
-3- confirm password : deja&amp;123&amp;
-4- national ID : 12345678912345
-5- email : khadija.mostafa@gmail.com
-6- phone :01284751822</t>
-  </si>
-  <si>
-    <t>1- enter username in the textfield username .
-2- enter password in the textfield password .
-3- enter confirm password in the textfield confirm password .
-4- enter national ID in the textfield national ID .
-5- enter email in the textfield email .
-6- enter phone in the textfield phone .
-7- leave staff id not selected .
-8-leave staff ID textfield empty.
-9- press on the button Register.
-10- click on close icon  in the pop up message .</t>
   </si>
   <si>
     <t>validate that Username field must contain numbers .</t>
@@ -769,10 +703,6 @@
   </si>
   <si>
     <t>validate that customer phone Field shall 
-accept length 6.</t>
-  </si>
-  <si>
-    <t>validate that customer phone Field shall 
 accept length 5.</t>
   </si>
   <si>
@@ -801,10 +731,6 @@
 5- email : khadija.mostafa@gmail.com
 6- phone :01284751820
 7- Staff id : 12345</t>
-  </si>
-  <si>
-    <t>validate that customer phone Field shall not
-accept characters</t>
   </si>
   <si>
     <t>1-user name : KhadijaMostafa93
@@ -988,12 +914,6 @@
 </t>
   </si>
   <si>
-    <t>BANK_SYS_TC_Reg_R050</t>
-  </si>
-  <si>
-    <t>BANK_SYS_TC_Reg_R051</t>
-  </si>
-  <si>
     <t>BANK_SYS_SRS_Reg_R032</t>
   </si>
   <si>
@@ -1040,6 +960,89 @@
   <si>
     <t>validate that no availability to register with 
 an exist admin data (admin register twice).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+error messgae in the form of pop up shall be displayed with context"  invalid format of data." beyound the username field in red color. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+error messgae in the form of pop up shall be displayed with context" length must be between 3:32" beyound the username field in red color. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+error messgae in the form of pop up shall be displayed with context"  invalid format of data."  beyound the username field in red color. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+error messgae in the form of pop up shall be displayed with context"  invalid format of data."  beyound the password field in red color. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+error messgae in the form of pop up shall be displayed with context"length must be between 8:12."  beyound the password field in red color. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+error messgae in the form of pop up shall be displayed with context"length must be between 8:12."  beyound the password field in red color. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+error messgae in the form of pop up shall be displayed with context"invalid format of data."  beyound the password field in red color. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+error messgae in the form of pop up shall be displayed with context"length must be 14."  beyound the national id  field in red color.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+error messgae in the form of pop up shall be displayed with context"invalid data format."  beyound the national id  field in red color. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+error messgae in the form of pop up shall be displayed with context"invalid data format."  beyound the phone  field in red color. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">error messgae in the form of pop up shall be displayed with context "max length must be 20 "  beyound the phone  field in red color. </t>
+  </si>
+  <si>
+    <t>validate that customer staff id Field shall 
+accept length 6.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">error messgae in the form of pop up shall be displayed with context" max length must be 6 "  beyound the staff id   field in red color. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">error messgae in the form of pop up shall be displayed with context" invalid format of data. "  beyound the staff id   field in red color. </t>
+  </si>
+  <si>
+    <t>validate that  admin staff id Field shall not
+accept characters</t>
+  </si>
+  <si>
+    <t>validate that admin staff id  Field shall not
+accept characters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">error messgae in the form of pop up shall be displayed with context" invalid format of data "  beyound the verification code   field in red color. </t>
+  </si>
+  <si>
+    <t>error messgae in the form of pop up shall be displayed with context" invalid format of data." beyound the verification code field in red color.</t>
+  </si>
+  <si>
+    <t>error messgae in the form of pop up shall be displayed with context"this field is mandatory." beyound the username field 
+in red color.</t>
+  </si>
+  <si>
+    <t>error messgae in the form of pop up shall be displayed with context"this field is mandatory." beyound the staff id  field 
+in red color.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">error messgae in the form of pop up shall be displayed with context"  invalid format of data." with ok button and close icon. </t>
   </si>
 </sst>
 </file>
@@ -1553,10 +1556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L59"/>
+  <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1690,7 +1693,7 @@
         <v>21</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E9" s="21" t="s">
         <v>22</v>
@@ -1745,7 +1748,7 @@
         <v>37</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E11" s="18" t="s">
         <v>38</v>
@@ -1765,22 +1768,22 @@
     </row>
     <row r="12" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B12" s="19" t="s">
         <v>40</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E12" s="18" t="s">
         <v>22</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>41</v>
+        <v>198</v>
       </c>
       <c r="H12" s="20" t="s">
         <v>23</v>
@@ -1794,22 +1797,22 @@
     </row>
     <row r="13" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="E13" s="18" t="s">
         <v>22</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="H13" s="20" t="s">
         <v>23</v>
@@ -1823,16 +1826,16 @@
     </row>
     <row r="14" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="E14" s="18" t="s">
         <v>22</v>
@@ -1852,22 +1855,22 @@
     </row>
     <row r="15" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E15" s="18" t="s">
         <v>22</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>41</v>
+        <v>199</v>
       </c>
       <c r="H15" s="20" t="s">
         <v>23</v>
@@ -1881,22 +1884,22 @@
     </row>
     <row r="16" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="D16" s="18" t="s">
         <v>148</v>
-      </c>
-      <c r="B16" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>158</v>
       </c>
       <c r="E16" s="18" t="s">
         <v>22</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>41</v>
+        <v>199</v>
       </c>
       <c r="H16" s="20" t="s">
         <v>23</v>
@@ -1906,16 +1909,16 @@
     </row>
     <row r="17" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="E17" s="18" t="s">
         <v>22</v>
@@ -1931,16 +1934,16 @@
     </row>
     <row r="18" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="E18" s="18" t="s">
         <v>22</v>
@@ -1956,22 +1959,22 @@
     </row>
     <row r="19" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="18" t="s">
         <v>53</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>63</v>
       </c>
       <c r="E19" s="18" t="s">
         <v>22</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>41</v>
+        <v>200</v>
       </c>
       <c r="H19" s="20" t="s">
         <v>23</v>
@@ -1985,22 +1988,22 @@
     </row>
     <row r="20" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="E20" s="18" t="s">
         <v>22</v>
       </c>
       <c r="F20" s="18" t="s">
-        <v>41</v>
+        <v>200</v>
       </c>
       <c r="H20" s="20" t="s">
         <v>23</v>
@@ -2014,22 +2017,22 @@
     </row>
     <row r="21" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>49</v>
+        <v>97</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="F21" s="18" t="s">
-        <v>44</v>
+        <v>201</v>
       </c>
       <c r="H21" s="20" t="s">
         <v>23</v>
@@ -2043,22 +2046,22 @@
     </row>
     <row r="22" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>58</v>
+        <v>98</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="F22" s="18" t="s">
-        <v>44</v>
+        <v>201</v>
       </c>
       <c r="H22" s="20" t="s">
         <v>23</v>
@@ -2071,23 +2074,23 @@
       </c>
     </row>
     <row r="23" spans="1:10" ht="165" x14ac:dyDescent="0.25">
-      <c r="A23" s="18" t="s">
-        <v>52</v>
+      <c r="A23" s="22" t="s">
+        <v>47</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F23" s="18" t="s">
-        <v>76</v>
+        <v>201</v>
       </c>
       <c r="H23" s="20" t="s">
         <v>23</v>
@@ -2100,23 +2103,23 @@
       </c>
     </row>
     <row r="24" spans="1:10" ht="165" x14ac:dyDescent="0.25">
-      <c r="A24" s="18" t="s">
-        <v>52</v>
+      <c r="A24" s="22" t="s">
+        <v>47</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F24" s="18" t="s">
-        <v>76</v>
+        <v>201</v>
       </c>
       <c r="H24" s="20" t="s">
         <v>23</v>
@@ -2130,22 +2133,22 @@
     </row>
     <row r="25" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>109</v>
+        <v>72</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F25" s="18" t="s">
-        <v>76</v>
+        <v>201</v>
       </c>
       <c r="H25" s="20" t="s">
         <v>23</v>
@@ -2159,22 +2162,22 @@
     </row>
     <row r="26" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F26" s="18" t="s">
-        <v>76</v>
+        <v>201</v>
       </c>
       <c r="H26" s="20" t="s">
         <v>23</v>
@@ -2188,22 +2191,22 @@
     </row>
     <row r="27" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F27" s="18" t="s">
-        <v>76</v>
+        <v>202</v>
       </c>
       <c r="H27" s="20" t="s">
         <v>23</v>
@@ -2217,22 +2220,22 @@
     </row>
     <row r="28" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F28" s="18" t="s">
-        <v>76</v>
+        <v>32</v>
       </c>
       <c r="H28" s="20" t="s">
         <v>23</v>
@@ -2245,49 +2248,49 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="165" x14ac:dyDescent="0.25">
-      <c r="A29" s="22" t="s">
+      <c r="A29" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="F29" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H29" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="I29" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="J29" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="B29" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="C29" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="D29" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="E29" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="F29" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="H29" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="I29" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J29" s="20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="165" x14ac:dyDescent="0.25">
-      <c r="A30" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="B30" s="19" t="s">
-        <v>102</v>
-      </c>
       <c r="C30" s="18" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F30" s="18" t="s">
         <v>32</v>
@@ -2304,19 +2307,19 @@
     </row>
     <row r="31" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F31" s="18" t="s">
         <v>32</v>
@@ -2333,22 +2336,22 @@
     </row>
     <row r="32" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F32" s="18" t="s">
-        <v>32</v>
+        <v>203</v>
       </c>
       <c r="H32" s="20" t="s">
         <v>23</v>
@@ -2362,22 +2365,22 @@
     </row>
     <row r="33" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="E33" s="18" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F33" s="18" t="s">
-        <v>32</v>
+        <v>204</v>
       </c>
       <c r="H33" s="20" t="s">
         <v>23</v>
@@ -2391,22 +2394,22 @@
     </row>
     <row r="34" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>92</v>
+        <v>115</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="E34" s="18" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F34" s="18" t="s">
-        <v>76</v>
+        <v>205</v>
       </c>
       <c r="H34" s="20" t="s">
         <v>23</v>
@@ -2420,22 +2423,22 @@
     </row>
     <row r="35" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F35" s="18" t="s">
-        <v>76</v>
+        <v>205</v>
       </c>
       <c r="H35" s="20" t="s">
         <v>23</v>
@@ -2449,22 +2452,22 @@
     </row>
     <row r="36" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>115</v>
+      </c>
+      <c r="B36" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="B36" s="19" t="s">
-        <v>135</v>
-      </c>
       <c r="C36" s="18" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F36" s="18" t="s">
-        <v>76</v>
+        <v>113</v>
       </c>
       <c r="H36" s="20" t="s">
         <v>23</v>
@@ -2478,22 +2481,22 @@
     </row>
     <row r="37" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F37" s="18" t="s">
-        <v>76</v>
+        <v>206</v>
       </c>
       <c r="H37" s="20" t="s">
         <v>23</v>
@@ -2507,22 +2510,22 @@
     </row>
     <row r="38" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F38" s="18" t="s">
-        <v>123</v>
+        <v>206</v>
       </c>
       <c r="H38" s="20" t="s">
         <v>23</v>
@@ -2536,51 +2539,51 @@
     </row>
     <row r="39" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B39" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="E39" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="F39" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="H39" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="I39" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="J39" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="B40" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="C39" s="18" t="s">
+      <c r="C40" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="D39" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="E39" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="F39" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="H39" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="I39" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J39" s="20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="165" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>126</v>
-      </c>
-      <c r="B40" s="19" t="s">
-        <v>152</v>
-      </c>
-      <c r="C40" s="18" t="s">
-        <v>129</v>
-      </c>
       <c r="D40" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F40" s="18" t="s">
-        <v>76</v>
+        <v>207</v>
       </c>
       <c r="H40" s="20" t="s">
         <v>23</v>
@@ -2594,22 +2597,22 @@
     </row>
     <row r="41" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D41" s="18" t="s">
         <v>139</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F41" s="18" t="s">
-        <v>76</v>
+        <v>113</v>
       </c>
       <c r="H41" s="20" t="s">
         <v>23</v>
@@ -2621,24 +2624,24 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="23" t="s">
-        <v>130</v>
+    <row r="42" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>133</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D42" s="18" t="s">
         <v>140</v>
       </c>
       <c r="E42" s="18" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F42" s="18" t="s">
-        <v>76</v>
+        <v>113</v>
       </c>
       <c r="H42" s="20" t="s">
         <v>23</v>
@@ -2652,22 +2655,22 @@
     </row>
     <row r="43" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="C43" s="18" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="E43" s="18" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F43" s="18" t="s">
-        <v>123</v>
+        <v>208</v>
       </c>
       <c r="H43" s="20" t="s">
         <v>23</v>
@@ -2681,22 +2684,22 @@
     </row>
     <row r="44" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="C44" s="18" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="E44" s="18" t="s">
-        <v>83</v>
+        <v>158</v>
       </c>
       <c r="F44" s="18" t="s">
-        <v>123</v>
+        <v>210</v>
       </c>
       <c r="H44" s="20" t="s">
         <v>23</v>
@@ -2710,22 +2713,22 @@
     </row>
     <row r="45" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="C45" s="18" t="s">
-        <v>146</v>
+        <v>209</v>
       </c>
       <c r="D45" s="18" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E45" s="18" t="s">
-        <v>83</v>
+        <v>158</v>
       </c>
       <c r="F45" s="18" t="s">
-        <v>76</v>
+        <v>160</v>
       </c>
       <c r="H45" s="20" t="s">
         <v>23</v>
@@ -2739,22 +2742,22 @@
     </row>
     <row r="46" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="C46" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="D46" s="18" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="E46" s="18" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="F46" s="18" t="s">
-        <v>76</v>
+        <v>160</v>
       </c>
       <c r="H46" s="20" t="s">
         <v>23</v>
@@ -2768,22 +2771,22 @@
     </row>
     <row r="47" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="C47" s="18" t="s">
-        <v>162</v>
+        <v>213</v>
       </c>
       <c r="D47" s="18" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="E47" s="18" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="F47" s="18" t="s">
-        <v>172</v>
+        <v>211</v>
       </c>
       <c r="H47" s="20" t="s">
         <v>23</v>
@@ -2797,22 +2800,22 @@
     </row>
     <row r="48" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="C48" s="18" t="s">
-        <v>163</v>
+        <v>212</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="E48" s="18" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="F48" s="18" t="s">
-        <v>172</v>
+        <v>211</v>
       </c>
       <c r="H48" s="20" t="s">
         <v>23</v>
@@ -2826,138 +2829,138 @@
     </row>
     <row r="49" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>147</v>
+        <v>27</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="C49" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="D49" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="E49" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="F49" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="H49" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="I49" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="J49" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="177" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>165</v>
+      </c>
+      <c r="B50" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="C50" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="D50" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E50" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="F50" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="H50" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="I50" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="J50" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="177" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>165</v>
+      </c>
+      <c r="B51" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="C51" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="D51" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E51" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="F51" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="H51" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="I51" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="J51" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="180" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>165</v>
+      </c>
+      <c r="B52" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="C52" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="D52" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="E52" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="D49" s="18" t="s">
+      <c r="F52" s="18" t="s">
         <v>168</v>
       </c>
-      <c r="E49" s="18" t="s">
+      <c r="H52" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="I52" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="J52" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="180" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>165</v>
+      </c>
+      <c r="B53" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="C53" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="F49" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="H49" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="I49" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J49" s="20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="165" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>147</v>
-      </c>
-      <c r="B50" s="19" t="s">
-        <v>190</v>
-      </c>
-      <c r="C50" s="18" t="s">
+      <c r="D53" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="E53" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="D50" s="18" t="s">
-        <v>169</v>
-      </c>
-      <c r="E50" s="18" t="s">
-        <v>170</v>
-      </c>
-      <c r="F50" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="H50" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="I50" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J50" s="20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="165" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>27</v>
-      </c>
-      <c r="B51" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="C51" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="D51" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="E51" s="18" t="s">
-        <v>170</v>
-      </c>
-      <c r="F51" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="H51" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="I51" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J51" s="20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" ht="177" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>177</v>
-      </c>
-      <c r="B52" s="19" t="s">
-        <v>192</v>
-      </c>
-      <c r="C52" s="18" t="s">
-        <v>173</v>
-      </c>
-      <c r="D52" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="E52" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="F52" s="18" t="s">
-        <v>176</v>
-      </c>
-      <c r="H52" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="I52" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J52" s="20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" ht="177" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>177</v>
-      </c>
-      <c r="B53" s="19" t="s">
-        <v>193</v>
-      </c>
-      <c r="C53" s="18" t="s">
-        <v>181</v>
-      </c>
-      <c r="D53" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="E53" s="18" t="s">
-        <v>175</v>
-      </c>
       <c r="F53" s="18" t="s">
-        <v>76</v>
+        <v>215</v>
       </c>
       <c r="H53" s="20" t="s">
         <v>23</v>
@@ -2971,109 +2974,109 @@
     </row>
     <row r="54" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="B54" s="19" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="C54" s="18" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="D54" s="18" t="s">
-        <v>165</v>
+        <v>193</v>
       </c>
       <c r="E54" s="18" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="F54" s="18" t="s">
-        <v>180</v>
-      </c>
-      <c r="H54" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="I54" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J54" s="20" t="s">
+        <v>216</v>
+      </c>
+      <c r="H54" t="s">
+        <v>23</v>
+      </c>
+      <c r="I54" t="s">
+        <v>24</v>
+      </c>
+      <c r="J54" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>177</v>
+        <v>191</v>
       </c>
       <c r="B55" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="C55" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="D55" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="E55" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="F55" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="H55" t="s">
+        <v>23</v>
+      </c>
+      <c r="I55" t="s">
+        <v>24</v>
+      </c>
+      <c r="J55" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="B56" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="C56" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="D56" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="E56" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="F56" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="H56" t="s">
+        <v>23</v>
+      </c>
+      <c r="I56" t="s">
+        <v>24</v>
+      </c>
+      <c r="J56" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="B57" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="C57" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="D57" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="E57" s="18" t="s">
         <v>195</v>
       </c>
-      <c r="C55" s="18" t="s">
-        <v>182</v>
-      </c>
-      <c r="D55" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="E55" s="18" t="s">
-        <v>179</v>
-      </c>
-      <c r="F55" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="H55" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="I55" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J55" s="20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" ht="180" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>204</v>
-      </c>
-      <c r="B56" t="s">
-        <v>196</v>
-      </c>
-      <c r="C56" s="18" t="s">
-        <v>197</v>
-      </c>
-      <c r="D56" s="18" t="s">
-        <v>207</v>
-      </c>
-      <c r="E56" s="18" t="s">
-        <v>198</v>
-      </c>
-      <c r="F56" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="H56" t="s">
-        <v>23</v>
-      </c>
-      <c r="I56" t="s">
-        <v>24</v>
-      </c>
-      <c r="J56" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" ht="180" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>205</v>
-      </c>
-      <c r="B57" t="s">
-        <v>199</v>
-      </c>
-      <c r="C57" s="18" t="s">
-        <v>206</v>
-      </c>
-      <c r="D57" s="18" t="s">
-        <v>200</v>
-      </c>
-      <c r="E57" s="18" t="s">
-        <v>201</v>
-      </c>
       <c r="F57" s="18" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="H57" t="s">
         <v>23</v>
@@ -3082,64 +3085,6 @@
         <v>24</v>
       </c>
       <c r="J57" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="23" t="s">
-        <v>177</v>
-      </c>
-      <c r="B58" t="s">
-        <v>202</v>
-      </c>
-      <c r="C58" s="18" t="s">
-        <v>210</v>
-      </c>
-      <c r="D58" s="18" t="s">
-        <v>200</v>
-      </c>
-      <c r="E58" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="F58" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="H58" t="s">
-        <v>23</v>
-      </c>
-      <c r="I58" t="s">
-        <v>24</v>
-      </c>
-      <c r="J58" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="23" t="s">
-        <v>177</v>
-      </c>
-      <c r="B59" t="s">
-        <v>203</v>
-      </c>
-      <c r="C59" s="18" t="s">
-        <v>211</v>
-      </c>
-      <c r="D59" s="18" t="s">
-        <v>208</v>
-      </c>
-      <c r="E59" s="18" t="s">
-        <v>209</v>
-      </c>
-      <c r="F59" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="H59" t="s">
-        <v>23</v>
-      </c>
-      <c r="I59" t="s">
-        <v>24</v>
-      </c>
-      <c r="J59" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update srs and reg module TCs with username field constraints
</commit_message>
<xml_diff>
--- a/Testing/Test Cases/Registeration TC.xlsx
+++ b/Testing/Test Cases/Registeration TC.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="220">
   <si>
     <t>Project Name:</t>
   </si>
@@ -211,18 +211,12 @@
     <t>BANK_SYS_TC_Reg_R007</t>
   </si>
   <si>
-    <t>validate that Username field must contain numbers .</t>
-  </si>
-  <si>
     <t>1-user name : KhadijaMostafa
 2- passsword : deja&amp;123&amp;
 3- confirm password : deja&amp;123&amp;
 4- national ID : 12345678912345
 5- email : khadija.mostafa@gmail.com
 6- phone :01284751820</t>
-  </si>
-  <si>
-    <t>validate that Username field must contain characters  .</t>
   </si>
   <si>
     <t>1-user name : 123456789
@@ -1043,6 +1037,16 @@
   </si>
   <si>
     <t xml:space="preserve">error messgae in the form of pop up shall be displayed with context"  invalid format of data." with ok button and close icon. </t>
+  </si>
+  <si>
+    <t>validate that Username field must contain characters not numbers only  .</t>
+  </si>
+  <si>
+    <t>validate that Username field can accept characters only.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customer shall be redirected to verification code page successfully .
+</t>
   </si>
 </sst>
 </file>
@@ -1558,8 +1562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1783,7 +1787,7 @@
         <v>22</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="H12" s="20" t="s">
         <v>23</v>
@@ -1803,16 +1807,16 @@
         <v>45</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E13" s="18" t="s">
         <v>22</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H13" s="20" t="s">
         <v>23</v>
@@ -1832,10 +1836,10 @@
         <v>46</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E14" s="18" t="s">
         <v>22</v>
@@ -1861,16 +1865,16 @@
         <v>49</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E15" s="18" t="s">
         <v>22</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="H15" s="20" t="s">
         <v>23</v>
@@ -1884,22 +1888,22 @@
     </row>
     <row r="16" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E16" s="18" t="s">
         <v>22</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="H16" s="20" t="s">
         <v>23</v>
@@ -1909,16 +1913,16 @@
     </row>
     <row r="17" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C17" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="D17" s="18" t="s">
         <v>147</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>149</v>
       </c>
       <c r="E17" s="18" t="s">
         <v>22</v>
@@ -1934,16 +1938,16 @@
     </row>
     <row r="18" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E18" s="18" t="s">
         <v>22</v>
@@ -1962,19 +1966,19 @@
         <v>48</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>52</v>
+        <v>217</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E19" s="18" t="s">
         <v>22</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H19" s="20" t="s">
         <v>23</v>
@@ -1991,19 +1995,19 @@
         <v>48</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C20" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="D20" s="18" t="s">
         <v>50</v>
-      </c>
-      <c r="D20" s="18" t="s">
-        <v>51</v>
       </c>
       <c r="E20" s="18" t="s">
         <v>22</v>
       </c>
       <c r="F20" s="18" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
       <c r="H20" s="20" t="s">
         <v>23</v>
@@ -2020,19 +2024,19 @@
         <v>47</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F21" s="18" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H21" s="20" t="s">
         <v>23</v>
@@ -2049,19 +2053,19 @@
         <v>47</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F22" s="18" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H22" s="20" t="s">
         <v>23</v>
@@ -2078,19 +2082,19 @@
         <v>47</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F23" s="18" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H23" s="20" t="s">
         <v>23</v>
@@ -2107,19 +2111,19 @@
         <v>47</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F24" s="18" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H24" s="20" t="s">
         <v>23</v>
@@ -2136,19 +2140,19 @@
         <v>47</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C25" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D25" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="E25" s="18" t="s">
-        <v>73</v>
-      </c>
       <c r="F25" s="18" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H25" s="20" t="s">
         <v>23</v>
@@ -2165,19 +2169,19 @@
         <v>47</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F26" s="18" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H26" s="20" t="s">
         <v>23</v>
@@ -2191,22 +2195,22 @@
     </row>
     <row r="27" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F27" s="18" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="H27" s="20" t="s">
         <v>23</v>
@@ -2220,19 +2224,19 @@
     </row>
     <row r="28" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F28" s="18" t="s">
         <v>32</v>
@@ -2249,19 +2253,19 @@
     </row>
     <row r="29" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F29" s="18" t="s">
         <v>32</v>
@@ -2278,19 +2282,19 @@
     </row>
     <row r="30" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B30" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="C30" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="D30" s="18" t="s">
-        <v>94</v>
-      </c>
       <c r="E30" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F30" s="18" t="s">
         <v>32</v>
@@ -2307,19 +2311,19 @@
     </row>
     <row r="31" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F31" s="18" t="s">
         <v>32</v>
@@ -2336,22 +2340,22 @@
     </row>
     <row r="32" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F32" s="18" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H32" s="20" t="s">
         <v>23</v>
@@ -2365,22 +2369,22 @@
     </row>
     <row r="33" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E33" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F33" s="18" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H33" s="20" t="s">
         <v>23</v>
@@ -2394,22 +2398,22 @@
     </row>
     <row r="34" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E34" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F34" s="18" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="H34" s="20" t="s">
         <v>23</v>
@@ -2423,22 +2427,22 @@
     </row>
     <row r="35" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F35" s="18" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="H35" s="20" t="s">
         <v>23</v>
@@ -2452,22 +2456,22 @@
     </row>
     <row r="36" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F36" s="18" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H36" s="20" t="s">
         <v>23</v>
@@ -2481,22 +2485,22 @@
     </row>
     <row r="37" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>114</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="D37" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="B37" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="C37" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>118</v>
-      </c>
       <c r="E37" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F37" s="18" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H37" s="20" t="s">
         <v>23</v>
@@ -2510,22 +2514,22 @@
     </row>
     <row r="38" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C38" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="D38" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="D38" s="18" t="s">
-        <v>121</v>
-      </c>
       <c r="E38" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F38" s="18" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H38" s="20" t="s">
         <v>23</v>
@@ -2539,22 +2543,22 @@
     </row>
     <row r="39" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E39" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F39" s="18" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H39" s="20" t="s">
         <v>23</v>
@@ -2568,22 +2572,22 @@
     </row>
     <row r="40" spans="1:10" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="23" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F40" s="18" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H40" s="20" t="s">
         <v>23</v>
@@ -2597,22 +2601,22 @@
     </row>
     <row r="41" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D41" s="18" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F41" s="18" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H41" s="20" t="s">
         <v>23</v>
@@ -2626,22 +2630,22 @@
     </row>
     <row r="42" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>131</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="C42" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="B42" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="C42" s="18" t="s">
-        <v>135</v>
-      </c>
       <c r="D42" s="18" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E42" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F42" s="18" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H42" s="20" t="s">
         <v>23</v>
@@ -2655,22 +2659,22 @@
     </row>
     <row r="43" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C43" s="18" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E43" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F43" s="18" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H43" s="20" t="s">
         <v>23</v>
@@ -2684,22 +2688,22 @@
     </row>
     <row r="44" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C44" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="D44" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="D44" s="18" t="s">
-        <v>153</v>
-      </c>
       <c r="E44" s="18" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F44" s="18" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="H44" s="20" t="s">
         <v>23</v>
@@ -2713,22 +2717,22 @@
     </row>
     <row r="45" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C45" s="18" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D45" s="18" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E45" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="F45" s="18" t="s">
         <v>158</v>
-      </c>
-      <c r="F45" s="18" t="s">
-        <v>160</v>
       </c>
       <c r="H45" s="20" t="s">
         <v>23</v>
@@ -2742,22 +2746,22 @@
     </row>
     <row r="46" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C46" s="18" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D46" s="18" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E46" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="F46" s="18" t="s">
         <v>158</v>
-      </c>
-      <c r="F46" s="18" t="s">
-        <v>160</v>
       </c>
       <c r="H46" s="20" t="s">
         <v>23</v>
@@ -2771,22 +2775,22 @@
     </row>
     <row r="47" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C47" s="18" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D47" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="E47" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="E47" s="18" t="s">
-        <v>158</v>
-      </c>
       <c r="F47" s="18" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="H47" s="20" t="s">
         <v>23</v>
@@ -2800,22 +2804,22 @@
     </row>
     <row r="48" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C48" s="18" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E48" s="18" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F48" s="18" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="H48" s="20" t="s">
         <v>23</v>
@@ -2832,19 +2836,19 @@
         <v>27</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D49" s="18" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E49" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="F49" s="18" t="s">
         <v>158</v>
-      </c>
-      <c r="F49" s="18" t="s">
-        <v>160</v>
       </c>
       <c r="H49" s="20" t="s">
         <v>23</v>
@@ -2858,22 +2862,22 @@
     </row>
     <row r="50" spans="1:10" ht="177" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D50" s="18" t="s">
         <v>41</v>
       </c>
       <c r="E50" s="18" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F50" s="18" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H50" s="20" t="s">
         <v>23</v>
@@ -2887,22 +2891,22 @@
     </row>
     <row r="51" spans="1:10" ht="177" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C51" s="18" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D51" s="18" t="s">
         <v>41</v>
       </c>
       <c r="E51" s="18" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F51" s="18" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H51" s="20" t="s">
         <v>23</v>
@@ -2916,22 +2920,22 @@
     </row>
     <row r="52" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>163</v>
+      </c>
+      <c r="B52" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="C52" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="D52" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="E52" s="18" t="s">
         <v>165</v>
       </c>
-      <c r="B52" s="19" t="s">
-        <v>180</v>
-      </c>
-      <c r="C52" s="18" t="s">
+      <c r="F52" s="18" t="s">
         <v>166</v>
-      </c>
-      <c r="D52" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="E52" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="F52" s="18" t="s">
-        <v>168</v>
       </c>
       <c r="H52" s="20" t="s">
         <v>23</v>
@@ -2945,22 +2949,22 @@
     </row>
     <row r="53" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>163</v>
+      </c>
+      <c r="B53" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="C53" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="D53" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="E53" s="18" t="s">
         <v>165</v>
       </c>
-      <c r="B53" s="19" t="s">
-        <v>181</v>
-      </c>
-      <c r="C53" s="18" t="s">
-        <v>170</v>
-      </c>
-      <c r="D53" s="18" t="s">
-        <v>162</v>
-      </c>
-      <c r="E53" s="18" t="s">
-        <v>167</v>
-      </c>
       <c r="F53" s="18" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H53" s="20" t="s">
         <v>23</v>
@@ -2974,22 +2978,22 @@
     </row>
     <row r="54" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B54" s="19" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C54" s="18" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D54" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E54" s="18" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F54" s="18" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H54" t="s">
         <v>23</v>
@@ -3003,22 +3007,22 @@
     </row>
     <row r="55" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B55" s="19" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C55" s="18" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D55" s="18" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E55" s="18" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F55" s="18" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H55" t="s">
         <v>23</v>
@@ -3032,22 +3036,22 @@
     </row>
     <row r="56" spans="1:10" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="23" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B56" s="19" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C56" s="18" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D56" s="18" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E56" s="18" t="s">
         <v>22</v>
       </c>
       <c r="F56" s="18" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H56" t="s">
         <v>23</v>
@@ -3061,22 +3065,22 @@
     </row>
     <row r="57" spans="1:10" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="23" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B57" s="19" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C57" s="18" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D57" s="18" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E57" s="18" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F57" s="18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H57" t="s">
         <v>23</v>

</xml_diff>